<commit_message>
updated test plan with first tests started
</commit_message>
<xml_diff>
--- a/Sprint 2/Test_Driven_Development/Testing_Plan.xlsx
+++ b/Sprint 2/Test_Driven_Development/Testing_Plan.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\AC31007-Agile\AC31007-AgileProject\Sprint 2\Test_Driven_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC4EDD0-BE40-4010-8CAC-CF85A8AA527B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A69B60B1-FC6B-4F56-9FF1-21B32804C4DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>DATE</t>
   </si>
@@ -58,7 +69,16 @@
     <t>add info about questionnaire correctly (title, description, researchers, contact info, agreement,...)</t>
   </si>
   <si>
-    <t>move on to questions page, correct info displayed on top</t>
+    <t>directs to a questionnaire page, correct info displayed on top</t>
+  </si>
+  <si>
+    <t>no method for redirecion, only placeholder data is displayed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>methods to get data from database are needed</t>
   </si>
   <si>
     <t>add info about questionnaire with empty fields</t>
@@ -67,13 +87,13 @@
     <t>error message, prompted to enter missing info</t>
   </si>
   <si>
-    <t>add question correctly (type, title, optional?, description)</t>
+    <t>add question correctly (type, title, optionality, description)</t>
   </si>
   <si>
     <t>question appears on the page with all associated data displayed</t>
   </si>
   <si>
-    <t>add question with ridiculously long text</t>
+    <t>add question with a lot of text</t>
   </si>
   <si>
     <t>rejected for being too long</t>
@@ -85,10 +105,19 @@
     <t>displayed with mandatory marking</t>
   </si>
   <si>
+    <t>Front-end can show mandatory or not with placeholder data.</t>
+  </si>
+  <si>
+    <t>Should test once backend done.</t>
+  </si>
+  <si>
     <t>add not mandatory question</t>
   </si>
   <si>
     <t>displayed without mandatory marking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front-end can show mandatory or not with placeholder data. </t>
   </si>
   <si>
     <t>add question with description</t>
@@ -97,13 +126,13 @@
     <t>question appears on the page with description</t>
   </si>
   <si>
+    <t>no frontend integration with database</t>
+  </si>
+  <si>
     <t>add question without description</t>
   </si>
   <si>
     <t>question appears on the page without  description</t>
-  </si>
-  <si>
-    <t>add question with missing mandatory info</t>
   </si>
   <si>
     <t>add open answer question</t>
@@ -112,54 +141,69 @@
     <t>question and empty text field appear on questionnaire</t>
   </si>
   <si>
-    <t>add multiple choice question</t>
+    <t>Front-end appears with placeholder data for now.</t>
   </si>
   <si>
-    <t>asked for further info (answer options, ...)</t>
-  </si>
-  <si>
-    <t>select MC question with one possible answer (radio button)</t>
+    <t>add MC question with one possible answer (radio buttons)</t>
   </si>
   <si>
     <t>question apprears with radio buttons for answers,
 only one answer can be selected</t>
   </si>
   <si>
-    <t>select MC question with multiple possible answers (checkboxes)</t>
+    <t>add MC question with multiple possible answers (checkboxes)</t>
   </si>
   <si>
     <t>question apprears with checkboxes for answers,
 0+ can be selected</t>
   </si>
   <si>
-    <t>add system usability scale</t>
+    <t>add question with system usability scale</t>
   </si>
   <si>
-    <t>asked for further info (scale, statements, ...)</t>
+    <t>question appears with a defined scale</t>
   </si>
   <si>
-    <t>select scale from 1-5</t>
+    <t xml:space="preserve">Not implemented </t>
   </si>
   <si>
-    <t>scale with five answer options between strongly aggree and strongly disagree</t>
+    <t>select open answer question</t>
   </si>
   <si>
-    <t>select scale from 1-10</t>
+    <t>a button to add a question is displayed</t>
   </si>
   <si>
-    <t>scale with ten answer options between strongly aggree and strongly disagree</t>
+    <t>method is not implemented</t>
   </si>
   <si>
-    <t>select scale and enter statement text</t>
+    <t>select MC question with one possible answer (radio buttons)</t>
+  </si>
+  <si>
+    <t>a box to enter answers options appears is displayed</t>
+  </si>
+  <si>
+    <t>select MC question with multiple possible answers (checkboxes)</t>
+  </si>
+  <si>
+    <t>select question with system usability scale</t>
+  </si>
+  <si>
+    <t>a box to enter range of scale and statements is displayed</t>
+  </si>
+  <si>
+    <t>add question with missing mandatory fields (title, optionality, type, answers)</t>
+  </si>
+  <si>
+    <t>no error handling methods created</t>
   </si>
   <si>
     <t>add another statement to existing scale</t>
   </si>
   <si>
-    <t>finish SUS with acceptable info</t>
+    <t>click finish questionnaire</t>
   </si>
   <si>
-    <t>dispalayed on questionnaire page with correct info and layout</t>
+    <t>questionnaire is saved, a title and  buttons (delete/send link/view) are displayed on the experiment page</t>
   </si>
 </sst>
 </file>
@@ -169,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -184,10 +228,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -254,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -274,28 +314,22 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,17 +567,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1018"/>
+  <dimension ref="A1:Y1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
@@ -628,9 +662,9 @@
       <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="9"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -651,8 +685,9 @@
       <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="7">
+        <f t="shared" ref="B4:B23" si="0">$B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -661,9 +696,9 @@
       <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -684,19 +719,28 @@
       <c r="Y4" s="2"/>
     </row>
     <row r="5" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6">
+        <v>44229</v>
+      </c>
       <c r="B5" s="7">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="9"/>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -719,17 +763,18 @@
     <row r="6" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>13</v>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>14</v>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -752,17 +797,18 @@
     <row r="7" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="7">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>15</v>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -785,17 +831,18 @@
     <row r="8" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>17</v>
+      <c r="C8" s="9" t="s">
+        <v>20</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>18</v>
+      <c r="D8" s="9" t="s">
+        <v>21</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -816,19 +863,28 @@
       <c r="Y8" s="2"/>
     </row>
     <row r="9" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6">
+        <v>44229</v>
+      </c>
       <c r="B9" s="7">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
+      <c r="C9" s="9" t="s">
+        <v>22</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>20</v>
+      <c r="D9" s="9" t="s">
+        <v>23</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -849,19 +905,28 @@
       <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6">
+        <v>44229</v>
+      </c>
       <c r="B10" s="7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>21</v>
+      <c r="C10" s="9" t="s">
+        <v>26</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>22</v>
+      <c r="D10" s="9" t="s">
+        <v>27</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="12"/>
+      <c r="E10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -882,19 +947,26 @@
       <c r="Y10" s="2"/>
     </row>
     <row r="11" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6">
+        <v>44229</v>
+      </c>
       <c r="B11" s="7">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>23</v>
+      <c r="C11" s="9" t="s">
+        <v>29</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>24</v>
+      <c r="D11" s="8" t="s">
+        <v>30</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="12"/>
+      <c r="E11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="9"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -915,19 +987,26 @@
       <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6">
+        <v>44229</v>
+      </c>
       <c r="B12" s="7">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>25</v>
+      <c r="C12" s="9" t="s">
+        <v>32</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>26</v>
+      <c r="D12" s="8" t="s">
+        <v>33</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="12"/>
+      <c r="E12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -948,19 +1027,26 @@
       <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6">
+        <v>44229</v>
+      </c>
       <c r="B13" s="7">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>27</v>
+      <c r="C13" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -981,19 +1067,26 @@
       <c r="Y13" s="2"/>
     </row>
     <row r="14" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="6">
+        <v>44229</v>
+      </c>
       <c r="B14" s="7">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>28</v>
+      <c r="C14" s="9" t="s">
+        <v>37</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>29</v>
+      <c r="D14" s="9" t="s">
+        <v>38</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="12"/>
+      <c r="E14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="9"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1014,19 +1107,26 @@
       <c r="Y14" s="2"/>
     </row>
     <row r="15" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6">
+        <v>44229</v>
+      </c>
       <c r="B15" s="7">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>30</v>
+      <c r="C15" s="9" t="s">
+        <v>39</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>31</v>
+      <c r="D15" s="9" t="s">
+        <v>40</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="12"/>
+      <c r="E15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="9"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1047,19 +1147,26 @@
       <c r="Y15" s="2"/>
     </row>
     <row r="16" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
+      <c r="A16" s="6">
+        <v>44229</v>
+      </c>
       <c r="B16" s="7">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>32</v>
+      <c r="C16" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="9"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1080,19 +1187,26 @@
       <c r="Y16" s="2"/>
     </row>
     <row r="17" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
+      <c r="A17" s="6">
+        <v>44229</v>
+      </c>
       <c r="B17" s="7">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>34</v>
+      <c r="C17" s="9" t="s">
+        <v>44</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>35</v>
+      <c r="D17" s="9" t="s">
+        <v>45</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="12"/>
+      <c r="E17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="9"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1113,19 +1227,26 @@
       <c r="Y17" s="2"/>
     </row>
     <row r="18" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
+      <c r="A18" s="6">
+        <v>44229</v>
+      </c>
       <c r="B18" s="7">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>36</v>
+      <c r="C18" s="9" t="s">
+        <v>47</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>37</v>
+      <c r="D18" s="9" t="s">
+        <v>48</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="12"/>
+      <c r="E18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="9"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1146,19 +1267,26 @@
       <c r="Y18" s="2"/>
     </row>
     <row r="19" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6">
+        <v>44229</v>
+      </c>
       <c r="B19" s="7">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>38</v>
+      <c r="C19" s="9" t="s">
+        <v>49</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>39</v>
+      <c r="D19" s="9" t="s">
+        <v>48</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="12"/>
+      <c r="E19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="9"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1179,19 +1307,26 @@
       <c r="Y19" s="2"/>
     </row>
     <row r="20" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6">
+        <v>44229</v>
+      </c>
       <c r="B20" s="7">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>40</v>
+      <c r="C20" s="9" t="s">
+        <v>50</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>41</v>
+      <c r="D20" s="9" t="s">
+        <v>51</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="12"/>
+      <c r="E20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="9"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1212,17 +1347,26 @@
       <c r="Y20" s="2"/>
     </row>
     <row r="21" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6">
+        <v>44229</v>
+      </c>
       <c r="B21" s="7">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>42</v>
+      <c r="C21" s="9" t="s">
+        <v>52</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="12"/>
+      <c r="D21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="9"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1245,15 +1389,16 @@
     <row r="22" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="7">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>43</v>
+      <c r="C22" s="9" t="s">
+        <v>54</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1276,17 +1421,18 @@
     <row r="23" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="7">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>44</v>
+      <c r="C23" s="9" t="s">
+        <v>55</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>45</v>
+      <c r="D23" s="9" t="s">
+        <v>56</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="12"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1308,12 +1454,12 @@
     </row>
     <row r="24" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="12"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1335,12 +1481,12 @@
     </row>
     <row r="25" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="12"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1362,12 +1508,12 @@
     </row>
     <row r="26" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="12"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1389,12 +1535,12 @@
     </row>
     <row r="27" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="12"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1414,14 +1560,14 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="12"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1441,14 +1587,14 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="12"/>
+    <row r="29" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -28144,46 +28290,19 @@
       <c r="X1017" s="2"/>
       <c r="Y1017" s="2"/>
     </row>
-    <row r="1018" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1018" s="2"/>
-      <c r="B1018" s="1"/>
-      <c r="C1018" s="2"/>
-      <c r="D1018" s="2"/>
-      <c r="E1018" s="2"/>
-      <c r="F1018" s="2"/>
-      <c r="G1018" s="2"/>
-      <c r="H1018" s="2"/>
-      <c r="I1018" s="2"/>
-      <c r="J1018" s="2"/>
-      <c r="K1018" s="2"/>
-      <c r="L1018" s="2"/>
-      <c r="M1018" s="2"/>
-      <c r="N1018" s="2"/>
-      <c r="O1018" s="2"/>
-      <c r="P1018" s="2"/>
-      <c r="Q1018" s="2"/>
-      <c r="R1018" s="2"/>
-      <c r="S1018" s="2"/>
-      <c r="T1018" s="2"/>
-      <c r="U1018" s="2"/>
-      <c r="V1018" s="2"/>
-      <c r="W1018" s="2"/>
-      <c r="X1018" s="2"/>
-      <c r="Y1018" s="2"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F29">
+  <conditionalFormatting sqref="F1:F28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F29">
+  <conditionalFormatting sqref="F3:F28">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="F3:F58" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F3:F57" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>